<commit_message>
app_mapabrechas-folium.pyCambiar ubicación de serie de tiempo y tabla de proyectos de nuevo nuevamente y faltan aun mas
</commit_message>
<xml_diff>
--- a/Proyectos_conteo_1.xlsx
+++ b/Proyectos_conteo_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://planeacionnacional-my.sharepoint.com/personal/ucd_dnp_gov_co/Documents/Repositorio UCD/Proyectos UCD/2024/P27-2024_Mapa_brechas/Codigo/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_10B5BAB91B484C0E62355476585DCE3A874FCF82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{808F8963-EC5F-4732-BD08-2C2BCFCC2D19}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_10B5BAB91B484C0E62355476585DCE3A874FCF82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27B26529-3F92-4437-B20D-F30AA3207B37}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4427,6 +4427,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4717,15 +4721,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G1330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="45.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="57.6640625" customWidth="1"/>
+    <col min="7" max="7" width="38.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -14244,7 +14246,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>522</v>
       </c>
@@ -23255,7 +23257,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="857" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="857" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A857" t="s">
         <v>961</v>
       </c>
@@ -31119,7 +31121,7 @@
   <autoFilter ref="A1:G1330" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="La Plata"/>
+        <filter val="Yondó"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>